<commit_message>
I've done loading and preproc function.
Trouble with sheets names is also allegedly rid off using RegEx.
</commit_message>
<xml_diff>
--- a/input/concentrations/ds.5p.ser/big_ser_test.xlsx
+++ b/input/concentrations/ds.5p.ser/big_ser_test.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\wannabecoder\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEVreplica\input\concentrations\ds.5p.ser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="11475" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="11475" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
-    <sheet name="input_k_constants_log10" sheetId="2" r:id="rId2"/>
-    <sheet name="input_concentrations" sheetId="3" r:id="rId3"/>
-    <sheet name="component_names" sheetId="4" r:id="rId4"/>
+    <sheet name="stoich_coeff" sheetId="1" r:id="rId1"/>
+    <sheet name="constants_log10" sheetId="2" r:id="rId2"/>
+    <sheet name="concentra" sheetId="3" r:id="rId3"/>
+    <sheet name="component" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -388,7 +388,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
python preproc mostly cleansed
</commit_message>
<xml_diff>
--- a/input/concentrations/ds.5p.ser/big_ser_test.xlsx
+++ b/input/concentrations/ds.5p.ser/big_ser_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\concentrations\ds.5p.ser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DE1643-52F7-4B59-BBBB-E63573D0D63C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CD738E-09BF-4A3B-B344-F0980D5CC797}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>tot</t>
   </si>
   <si>
-    <t>ser_num</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>ass</t>
+  </si>
+  <si>
+    <t>series</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -802,7 +802,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>9.9999999999999998E-20</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>8.5000000000000006E-5</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>8.5000000000000006E-5</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>